<commit_message>
Add information about world_pollution data
</commit_message>
<xml_diff>
--- a/data/world_pollution/world_co2_emissions_per_capita.xlsx
+++ b/data/world_pollution/world_co2_emissions_per_capita.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/twitter/Desktop/INFO201B/final-project-kje123/data/world_pollution/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C431BC3B-45C6-6542-AA33-B28340C4CCB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99CF0AEB-0FF5-744E-ADA1-B17B6F2BFBEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="API_EN.ATM.CO2E.PC_DS2_en_csv_v" sheetId="1" r:id="rId1"/>
@@ -343,9 +343,6 @@
     <t>CUB</t>
   </si>
   <si>
-    <t>Curacao</t>
-  </si>
-  <si>
     <t>CUW</t>
   </si>
   <si>
@@ -1631,6 +1628,9 @@
   </si>
   <si>
     <t>ZWE</t>
+  </si>
+  <si>
+    <t>Curaçao</t>
   </si>
 </sst>
 </file>
@@ -2472,10 +2472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BL269"/>
+  <dimension ref="A1:BK269"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="BB1" workbookViewId="0">
+      <selection activeCell="BK11" sqref="BK11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="39.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2487,7 +2487,7 @@
     <col min="5" max="64" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2495,7 +2495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2503,7 +2503,7 @@
         <v>43819</v>
       </c>
     </row>
-    <row r="5" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -2681,23 +2681,8 @@
       <c r="BG5">
         <v>2014</v>
       </c>
-      <c r="BH5">
-        <v>2015</v>
-      </c>
-      <c r="BI5">
-        <v>2016</v>
-      </c>
-      <c r="BJ5">
-        <v>2017</v>
-      </c>
-      <c r="BK5">
-        <v>2018</v>
-      </c>
-      <c r="BL5">
-        <v>2019</v>
-      </c>
     </row>
-    <row r="6" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -2798,7 +2783,7 @@
         <v>8.4100641779251095</v>
       </c>
     </row>
-    <row r="7" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -2977,7 +2962,7 @@
         <v>0.293946407148718</v>
       </c>
     </row>
-    <row r="8" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -3156,7 +3141,7 @@
         <v>1.2903067759556599</v>
       </c>
     </row>
-    <row r="9" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -3335,7 +3320,7 @@
         <v>1.97876331208568</v>
       </c>
     </row>
-    <row r="10" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -3424,7 +3409,7 @@
         <v>5.8329062148889701</v>
       </c>
     </row>
-    <row r="11" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -3603,7 +3588,7 @@
         <v>4.8869875132919498</v>
       </c>
     </row>
-    <row r="12" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -3782,7 +3767,7 @@
         <v>22.939606313099102</v>
       </c>
     </row>
-    <row r="13" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -3961,7 +3946,7 @@
         <v>4.7815077748743198</v>
       </c>
     </row>
-    <row r="14" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -4044,7 +4029,7 @@
         <v>1.8987193736581101</v>
       </c>
     </row>
-    <row r="15" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -4058,7 +4043,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -10480,10 +10465,10 @@
     </row>
     <row r="55" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
+        <v>536</v>
+      </c>
+      <c r="B55" t="s">
         <v>107</v>
-      </c>
-      <c r="B55" t="s">
-        <v>108</v>
       </c>
       <c r="C55" t="s">
         <v>9</v>
@@ -10503,10 +10488,10 @@
     </row>
     <row r="56" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
+        <v>108</v>
+      </c>
+      <c r="B56" t="s">
         <v>109</v>
-      </c>
-      <c r="B56" t="s">
-        <v>110</v>
       </c>
       <c r="C56" t="s">
         <v>9</v>
@@ -10682,10 +10667,10 @@
     </row>
     <row r="57" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
+        <v>110</v>
+      </c>
+      <c r="B57" t="s">
         <v>111</v>
-      </c>
-      <c r="B57" t="s">
-        <v>112</v>
       </c>
       <c r="C57" t="s">
         <v>9</v>
@@ -10861,10 +10846,10 @@
     </row>
     <row r="58" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
+        <v>112</v>
+      </c>
+      <c r="B58" t="s">
         <v>113</v>
-      </c>
-      <c r="B58" t="s">
-        <v>114</v>
       </c>
       <c r="C58" t="s">
         <v>9</v>
@@ -10944,10 +10929,10 @@
     </row>
     <row r="59" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
+        <v>114</v>
+      </c>
+      <c r="B59" t="s">
         <v>115</v>
-      </c>
-      <c r="B59" t="s">
-        <v>116</v>
       </c>
       <c r="C59" t="s">
         <v>9</v>
@@ -11030,10 +11015,10 @@
     </row>
     <row r="60" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
+        <v>116</v>
+      </c>
+      <c r="B60" t="s">
         <v>117</v>
-      </c>
-      <c r="B60" t="s">
-        <v>118</v>
       </c>
       <c r="C60" t="s">
         <v>9</v>
@@ -11209,10 +11194,10 @@
     </row>
     <row r="61" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
+        <v>118</v>
+      </c>
+      <c r="B61" t="s">
         <v>119</v>
-      </c>
-      <c r="B61" t="s">
-        <v>120</v>
       </c>
       <c r="C61" t="s">
         <v>9</v>
@@ -11388,10 +11373,10 @@
     </row>
     <row r="62" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
+        <v>120</v>
+      </c>
+      <c r="B62" t="s">
         <v>121</v>
-      </c>
-      <c r="B62" t="s">
-        <v>122</v>
       </c>
       <c r="C62" t="s">
         <v>9</v>
@@ -11567,10 +11552,10 @@
     </row>
     <row r="63" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
+        <v>122</v>
+      </c>
+      <c r="B63" t="s">
         <v>123</v>
-      </c>
-      <c r="B63" t="s">
-        <v>124</v>
       </c>
       <c r="C63" t="s">
         <v>9</v>
@@ -11746,10 +11731,10 @@
     </row>
     <row r="64" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
+        <v>124</v>
+      </c>
+      <c r="B64" t="s">
         <v>125</v>
-      </c>
-      <c r="B64" t="s">
-        <v>126</v>
       </c>
       <c r="C64" t="s">
         <v>9</v>
@@ -11925,10 +11910,10 @@
     </row>
     <row r="65" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
+        <v>126</v>
+      </c>
+      <c r="B65" t="s">
         <v>127</v>
-      </c>
-      <c r="B65" t="s">
-        <v>128</v>
       </c>
       <c r="C65" t="s">
         <v>9</v>
@@ -12104,10 +12089,10 @@
     </row>
     <row r="66" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
+        <v>128</v>
+      </c>
+      <c r="B66" t="s">
         <v>129</v>
-      </c>
-      <c r="B66" t="s">
-        <v>130</v>
       </c>
       <c r="C66" t="s">
         <v>9</v>
@@ -12283,10 +12268,10 @@
     </row>
     <row r="67" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
+        <v>130</v>
+      </c>
+      <c r="B67" t="s">
         <v>131</v>
-      </c>
-      <c r="B67" t="s">
-        <v>132</v>
       </c>
       <c r="C67" t="s">
         <v>9</v>
@@ -12462,10 +12447,10 @@
     </row>
     <row r="68" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
+        <v>132</v>
+      </c>
+      <c r="B68" t="s">
         <v>133</v>
-      </c>
-      <c r="B68" t="s">
-        <v>134</v>
       </c>
       <c r="C68" t="s">
         <v>9</v>
@@ -12545,10 +12530,10 @@
     </row>
     <row r="69" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
+        <v>134</v>
+      </c>
+      <c r="B69" t="s">
         <v>135</v>
-      </c>
-      <c r="B69" t="s">
-        <v>136</v>
       </c>
       <c r="C69" t="s">
         <v>9</v>
@@ -12628,10 +12613,10 @@
     </row>
     <row r="70" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
+        <v>136</v>
+      </c>
+      <c r="B70" t="s">
         <v>137</v>
-      </c>
-      <c r="B70" t="s">
-        <v>138</v>
       </c>
       <c r="C70" t="s">
         <v>9</v>
@@ -12807,10 +12792,10 @@
     </row>
     <row r="71" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
+        <v>138</v>
+      </c>
+      <c r="B71" t="s">
         <v>139</v>
-      </c>
-      <c r="B71" t="s">
-        <v>140</v>
       </c>
       <c r="C71" t="s">
         <v>9</v>
@@ -12986,10 +12971,10 @@
     </row>
     <row r="72" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
+        <v>140</v>
+      </c>
+      <c r="B72" t="s">
         <v>141</v>
-      </c>
-      <c r="B72" t="s">
-        <v>142</v>
       </c>
       <c r="C72" t="s">
         <v>9</v>
@@ -13072,10 +13057,10 @@
     </row>
     <row r="73" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
+        <v>142</v>
+      </c>
+      <c r="B73" t="s">
         <v>143</v>
-      </c>
-      <c r="B73" t="s">
-        <v>144</v>
       </c>
       <c r="C73" t="s">
         <v>9</v>
@@ -13140,10 +13125,10 @@
     </row>
     <row r="74" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
+        <v>144</v>
+      </c>
+      <c r="B74" t="s">
         <v>145</v>
-      </c>
-      <c r="B74" t="s">
-        <v>146</v>
       </c>
       <c r="C74" t="s">
         <v>9</v>
@@ -13319,10 +13304,10 @@
     </row>
     <row r="75" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
+        <v>146</v>
+      </c>
+      <c r="B75" t="s">
         <v>147</v>
-      </c>
-      <c r="B75" t="s">
-        <v>148</v>
       </c>
       <c r="C75" t="s">
         <v>9</v>
@@ -13402,10 +13387,10 @@
     </row>
     <row r="76" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
+        <v>148</v>
+      </c>
+      <c r="B76" t="s">
         <v>149</v>
-      </c>
-      <c r="B76" t="s">
-        <v>150</v>
       </c>
       <c r="C76" t="s">
         <v>9</v>
@@ -13581,10 +13566,10 @@
     </row>
     <row r="77" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
+        <v>150</v>
+      </c>
+      <c r="B77" t="s">
         <v>151</v>
-      </c>
-      <c r="B77" t="s">
-        <v>152</v>
       </c>
       <c r="C77" t="s">
         <v>9</v>
@@ -13760,10 +13745,10 @@
     </row>
     <row r="78" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
+        <v>152</v>
+      </c>
+      <c r="B78" t="s">
         <v>153</v>
-      </c>
-      <c r="B78" t="s">
-        <v>154</v>
       </c>
       <c r="C78" t="s">
         <v>9</v>
@@ -13939,10 +13924,10 @@
     </row>
     <row r="79" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
+        <v>154</v>
+      </c>
+      <c r="B79" t="s">
         <v>155</v>
-      </c>
-      <c r="B79" t="s">
-        <v>156</v>
       </c>
       <c r="C79" t="s">
         <v>9</v>
@@ -14118,10 +14103,10 @@
     </row>
     <row r="80" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
+        <v>156</v>
+      </c>
+      <c r="B80" t="s">
         <v>157</v>
-      </c>
-      <c r="B80" t="s">
-        <v>158</v>
       </c>
       <c r="C80" t="s">
         <v>9</v>
@@ -14297,10 +14282,10 @@
     </row>
     <row r="81" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
+        <v>158</v>
+      </c>
+      <c r="B81" t="s">
         <v>159</v>
-      </c>
-      <c r="B81" t="s">
-        <v>160</v>
       </c>
       <c r="C81" t="s">
         <v>9</v>
@@ -14476,10 +14461,10 @@
     </row>
     <row r="82" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
+        <v>160</v>
+      </c>
+      <c r="B82" t="s">
         <v>161</v>
-      </c>
-      <c r="B82" t="s">
-        <v>162</v>
       </c>
       <c r="C82" t="s">
         <v>9</v>
@@ -14655,10 +14640,10 @@
     </row>
     <row r="83" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
+        <v>162</v>
+      </c>
+      <c r="B83" t="s">
         <v>163</v>
-      </c>
-      <c r="B83" t="s">
-        <v>164</v>
       </c>
       <c r="C83" t="s">
         <v>9</v>
@@ -14738,10 +14723,10 @@
     </row>
     <row r="84" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
+        <v>164</v>
+      </c>
+      <c r="B84" t="s">
         <v>165</v>
-      </c>
-      <c r="B84" t="s">
-        <v>166</v>
       </c>
       <c r="C84" t="s">
         <v>9</v>
@@ -14917,10 +14902,10 @@
     </row>
     <row r="85" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
+        <v>166</v>
+      </c>
+      <c r="B85" t="s">
         <v>167</v>
-      </c>
-      <c r="B85" t="s">
-        <v>168</v>
       </c>
       <c r="C85" t="s">
         <v>9</v>
@@ -15096,10 +15081,10 @@
     </row>
     <row r="86" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
+        <v>168</v>
+      </c>
+      <c r="B86" t="s">
         <v>169</v>
-      </c>
-      <c r="B86" t="s">
-        <v>170</v>
       </c>
       <c r="C86" t="s">
         <v>9</v>
@@ -15179,10 +15164,10 @@
     </row>
     <row r="87" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
+        <v>170</v>
+      </c>
+      <c r="B87" t="s">
         <v>171</v>
-      </c>
-      <c r="B87" t="s">
-        <v>172</v>
       </c>
       <c r="C87" t="s">
         <v>9</v>
@@ -15358,10 +15343,10 @@
     </row>
     <row r="88" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
+        <v>172</v>
+      </c>
+      <c r="B88" t="s">
         <v>173</v>
-      </c>
-      <c r="B88" t="s">
-        <v>174</v>
       </c>
       <c r="C88" t="s">
         <v>9</v>
@@ -15537,10 +15522,10 @@
     </row>
     <row r="89" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
+        <v>174</v>
+      </c>
+      <c r="B89" t="s">
         <v>175</v>
-      </c>
-      <c r="B89" t="s">
-        <v>176</v>
       </c>
       <c r="C89" t="s">
         <v>9</v>
@@ -15716,10 +15701,10 @@
     </row>
     <row r="90" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
+        <v>176</v>
+      </c>
+      <c r="B90" t="s">
         <v>177</v>
-      </c>
-      <c r="B90" t="s">
-        <v>178</v>
       </c>
       <c r="C90" t="s">
         <v>9</v>
@@ -15895,10 +15880,10 @@
     </row>
     <row r="91" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
+        <v>178</v>
+      </c>
+      <c r="B91" t="s">
         <v>179</v>
-      </c>
-      <c r="B91" t="s">
-        <v>180</v>
       </c>
       <c r="C91" t="s">
         <v>9</v>
@@ -16074,10 +16059,10 @@
     </row>
     <row r="92" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
+        <v>180</v>
+      </c>
+      <c r="B92" t="s">
         <v>181</v>
-      </c>
-      <c r="B92" t="s">
-        <v>182</v>
       </c>
       <c r="C92" t="s">
         <v>9</v>
@@ -16253,10 +16238,10 @@
     </row>
     <row r="93" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
+        <v>182</v>
+      </c>
+      <c r="B93" t="s">
         <v>183</v>
-      </c>
-      <c r="B93" t="s">
-        <v>184</v>
       </c>
       <c r="C93" t="s">
         <v>9</v>
@@ -16432,10 +16417,10 @@
     </row>
     <row r="94" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
+        <v>184</v>
+      </c>
+      <c r="B94" t="s">
         <v>185</v>
-      </c>
-      <c r="B94" t="s">
-        <v>186</v>
       </c>
       <c r="C94" t="s">
         <v>9</v>
@@ -16611,10 +16596,10 @@
     </row>
     <row r="95" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
+        <v>186</v>
+      </c>
+      <c r="B95" t="s">
         <v>187</v>
-      </c>
-      <c r="B95" t="s">
-        <v>188</v>
       </c>
       <c r="C95" t="s">
         <v>9</v>
@@ -16790,10 +16775,10 @@
     </row>
     <row r="96" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
+        <v>188</v>
+      </c>
+      <c r="B96" t="s">
         <v>189</v>
-      </c>
-      <c r="B96" t="s">
-        <v>190</v>
       </c>
       <c r="C96" t="s">
         <v>9</v>
@@ -16969,10 +16954,10 @@
     </row>
     <row r="97" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
+        <v>190</v>
+      </c>
+      <c r="B97" t="s">
         <v>191</v>
-      </c>
-      <c r="B97" t="s">
-        <v>192</v>
       </c>
       <c r="C97" t="s">
         <v>9</v>
@@ -16983,10 +16968,10 @@
     </row>
     <row r="98" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
+        <v>192</v>
+      </c>
+      <c r="B98" t="s">
         <v>193</v>
-      </c>
-      <c r="B98" t="s">
-        <v>194</v>
       </c>
       <c r="C98" t="s">
         <v>9</v>
@@ -17162,10 +17147,10 @@
     </row>
     <row r="99" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
+        <v>194</v>
+      </c>
+      <c r="B99" t="s">
         <v>195</v>
-      </c>
-      <c r="B99" t="s">
-        <v>196</v>
       </c>
       <c r="C99" t="s">
         <v>9</v>
@@ -17341,10 +17326,10 @@
     </row>
     <row r="100" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
+        <v>196</v>
+      </c>
+      <c r="B100" t="s">
         <v>197</v>
-      </c>
-      <c r="B100" t="s">
-        <v>198</v>
       </c>
       <c r="C100" t="s">
         <v>9</v>
@@ -17520,10 +17505,10 @@
     </row>
     <row r="101" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
+        <v>198</v>
+      </c>
+      <c r="B101" t="s">
         <v>199</v>
-      </c>
-      <c r="B101" t="s">
-        <v>200</v>
       </c>
       <c r="C101" t="s">
         <v>9</v>
@@ -17699,10 +17684,10 @@
     </row>
     <row r="102" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
+        <v>200</v>
+      </c>
+      <c r="B102" t="s">
         <v>201</v>
-      </c>
-      <c r="B102" t="s">
-        <v>202</v>
       </c>
       <c r="C102" t="s">
         <v>9</v>
@@ -17878,10 +17863,10 @@
     </row>
     <row r="103" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
+        <v>202</v>
+      </c>
+      <c r="B103" t="s">
         <v>203</v>
-      </c>
-      <c r="B103" t="s">
-        <v>204</v>
       </c>
       <c r="C103" t="s">
         <v>9</v>
@@ -17961,10 +17946,10 @@
     </row>
     <row r="104" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
+        <v>204</v>
+      </c>
+      <c r="B104" t="s">
         <v>205</v>
-      </c>
-      <c r="B104" t="s">
-        <v>206</v>
       </c>
       <c r="C104" t="s">
         <v>9</v>
@@ -18140,10 +18125,10 @@
     </row>
     <row r="105" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
+        <v>206</v>
+      </c>
+      <c r="B105" t="s">
         <v>207</v>
-      </c>
-      <c r="B105" t="s">
-        <v>208</v>
       </c>
       <c r="C105" t="s">
         <v>9</v>
@@ -18319,10 +18304,10 @@
     </row>
     <row r="106" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
+        <v>208</v>
+      </c>
+      <c r="B106" t="s">
         <v>209</v>
-      </c>
-      <c r="B106" t="s">
-        <v>210</v>
       </c>
       <c r="C106" t="s">
         <v>9</v>
@@ -18498,10 +18483,10 @@
     </row>
     <row r="107" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
+        <v>210</v>
+      </c>
+      <c r="B107" t="s">
         <v>211</v>
-      </c>
-      <c r="B107" t="s">
-        <v>212</v>
       </c>
       <c r="C107" t="s">
         <v>9</v>
@@ -18677,10 +18662,10 @@
     </row>
     <row r="108" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
+        <v>212</v>
+      </c>
+      <c r="B108" t="s">
         <v>213</v>
-      </c>
-      <c r="B108" t="s">
-        <v>214</v>
       </c>
       <c r="C108" t="s">
         <v>9</v>
@@ -18856,10 +18841,10 @@
     </row>
     <row r="109" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
+        <v>214</v>
+      </c>
+      <c r="B109" t="s">
         <v>215</v>
-      </c>
-      <c r="B109" t="s">
-        <v>216</v>
       </c>
       <c r="C109" t="s">
         <v>9</v>
@@ -19035,10 +19020,10 @@
     </row>
     <row r="110" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
+        <v>216</v>
+      </c>
+      <c r="B110" t="s">
         <v>217</v>
-      </c>
-      <c r="B110" t="s">
-        <v>218</v>
       </c>
       <c r="C110" t="s">
         <v>9</v>
@@ -19214,10 +19199,10 @@
     </row>
     <row r="111" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
+        <v>218</v>
+      </c>
+      <c r="B111" t="s">
         <v>219</v>
-      </c>
-      <c r="B111" t="s">
-        <v>220</v>
       </c>
       <c r="C111" t="s">
         <v>9</v>
@@ -19393,10 +19378,10 @@
     </row>
     <row r="112" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
+        <v>220</v>
+      </c>
+      <c r="B112" t="s">
         <v>221</v>
-      </c>
-      <c r="B112" t="s">
-        <v>222</v>
       </c>
       <c r="C112" t="s">
         <v>9</v>
@@ -19407,10 +19392,10 @@
     </row>
     <row r="113" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
+        <v>222</v>
+      </c>
+      <c r="B113" t="s">
         <v>223</v>
-      </c>
-      <c r="B113" t="s">
-        <v>224</v>
       </c>
       <c r="C113" t="s">
         <v>9</v>
@@ -19586,10 +19571,10 @@
     </row>
     <row r="114" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
+        <v>224</v>
+      </c>
+      <c r="B114" t="s">
         <v>225</v>
-      </c>
-      <c r="B114" t="s">
-        <v>226</v>
       </c>
       <c r="C114" t="s">
         <v>9</v>
@@ -19600,10 +19585,10 @@
     </row>
     <row r="115" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
+        <v>226</v>
+      </c>
+      <c r="B115" t="s">
         <v>227</v>
-      </c>
-      <c r="B115" t="s">
-        <v>228</v>
       </c>
       <c r="C115" t="s">
         <v>9</v>
@@ -19779,10 +19764,10 @@
     </row>
     <row r="116" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
+        <v>228</v>
+      </c>
+      <c r="B116" t="s">
         <v>229</v>
-      </c>
-      <c r="B116" t="s">
-        <v>230</v>
       </c>
       <c r="C116" t="s">
         <v>9</v>
@@ -19958,10 +19943,10 @@
     </row>
     <row r="117" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
+        <v>230</v>
+      </c>
+      <c r="B117" t="s">
         <v>231</v>
-      </c>
-      <c r="B117" t="s">
-        <v>232</v>
       </c>
       <c r="C117" t="s">
         <v>9</v>
@@ -20137,10 +20122,10 @@
     </row>
     <row r="118" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
+        <v>232</v>
+      </c>
+      <c r="B118" t="s">
         <v>233</v>
-      </c>
-      <c r="B118" t="s">
-        <v>234</v>
       </c>
       <c r="C118" t="s">
         <v>9</v>
@@ -20316,10 +20301,10 @@
     </row>
     <row r="119" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
+        <v>234</v>
+      </c>
+      <c r="B119" t="s">
         <v>235</v>
-      </c>
-      <c r="B119" t="s">
-        <v>236</v>
       </c>
       <c r="C119" t="s">
         <v>9</v>
@@ -20495,10 +20480,10 @@
     </row>
     <row r="120" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
+        <v>236</v>
+      </c>
+      <c r="B120" t="s">
         <v>237</v>
-      </c>
-      <c r="B120" t="s">
-        <v>238</v>
       </c>
       <c r="C120" t="s">
         <v>9</v>
@@ -20674,10 +20659,10 @@
     </row>
     <row r="121" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
+        <v>238</v>
+      </c>
+      <c r="B121" t="s">
         <v>239</v>
-      </c>
-      <c r="B121" t="s">
-        <v>240</v>
       </c>
       <c r="C121" t="s">
         <v>9</v>
@@ -20853,10 +20838,10 @@
     </row>
     <row r="122" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
+        <v>240</v>
+      </c>
+      <c r="B122" t="s">
         <v>241</v>
-      </c>
-      <c r="B122" t="s">
-        <v>242</v>
       </c>
       <c r="C122" t="s">
         <v>9</v>
@@ -21032,10 +21017,10 @@
     </row>
     <row r="123" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
+        <v>242</v>
+      </c>
+      <c r="B123" t="s">
         <v>243</v>
-      </c>
-      <c r="B123" t="s">
-        <v>244</v>
       </c>
       <c r="C123" t="s">
         <v>9</v>
@@ -21211,10 +21196,10 @@
     </row>
     <row r="124" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
+        <v>244</v>
+      </c>
+      <c r="B124" t="s">
         <v>245</v>
-      </c>
-      <c r="B124" t="s">
-        <v>246</v>
       </c>
       <c r="C124" t="s">
         <v>9</v>
@@ -21294,10 +21279,10 @@
     </row>
     <row r="125" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
+        <v>246</v>
+      </c>
+      <c r="B125" t="s">
         <v>247</v>
-      </c>
-      <c r="B125" t="s">
-        <v>248</v>
       </c>
       <c r="C125" t="s">
         <v>9</v>
@@ -21473,10 +21458,10 @@
     </row>
     <row r="126" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
+        <v>248</v>
+      </c>
+      <c r="B126" t="s">
         <v>249</v>
-      </c>
-      <c r="B126" t="s">
-        <v>250</v>
       </c>
       <c r="C126" t="s">
         <v>9</v>
@@ -21556,10 +21541,10 @@
     </row>
     <row r="127" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
+        <v>250</v>
+      </c>
+      <c r="B127" t="s">
         <v>251</v>
-      </c>
-      <c r="B127" t="s">
-        <v>252</v>
       </c>
       <c r="C127" t="s">
         <v>9</v>
@@ -21735,10 +21720,10 @@
     </row>
     <row r="128" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
+        <v>252</v>
+      </c>
+      <c r="B128" t="s">
         <v>253</v>
-      </c>
-      <c r="B128" t="s">
-        <v>254</v>
       </c>
       <c r="C128" t="s">
         <v>9</v>
@@ -21911,10 +21896,10 @@
     </row>
     <row r="129" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
+        <v>254</v>
+      </c>
+      <c r="B129" t="s">
         <v>255</v>
-      </c>
-      <c r="B129" t="s">
-        <v>256</v>
       </c>
       <c r="C129" t="s">
         <v>9</v>
@@ -22090,10 +22075,10 @@
     </row>
     <row r="130" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
+        <v>256</v>
+      </c>
+      <c r="B130" t="s">
         <v>257</v>
-      </c>
-      <c r="B130" t="s">
-        <v>258</v>
       </c>
       <c r="C130" t="s">
         <v>9</v>
@@ -22269,10 +22254,10 @@
     </row>
     <row r="131" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
+        <v>258</v>
+      </c>
+      <c r="B131" t="s">
         <v>259</v>
-      </c>
-      <c r="B131" t="s">
-        <v>260</v>
       </c>
       <c r="C131" t="s">
         <v>9</v>
@@ -22439,10 +22424,10 @@
     </row>
     <row r="132" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
+        <v>260</v>
+      </c>
+      <c r="B132" t="s">
         <v>261</v>
-      </c>
-      <c r="B132" t="s">
-        <v>262</v>
       </c>
       <c r="C132" t="s">
         <v>9</v>
@@ -22618,10 +22603,10 @@
     </row>
     <row r="133" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
+        <v>262</v>
+      </c>
+      <c r="B133" t="s">
         <v>263</v>
-      </c>
-      <c r="B133" t="s">
-        <v>264</v>
       </c>
       <c r="C133" t="s">
         <v>9</v>
@@ -22797,10 +22782,10 @@
     </row>
     <row r="134" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
+        <v>264</v>
+      </c>
+      <c r="B134" t="s">
         <v>265</v>
-      </c>
-      <c r="B134" t="s">
-        <v>266</v>
       </c>
       <c r="C134" t="s">
         <v>9</v>
@@ -22976,10 +22961,10 @@
     </row>
     <row r="135" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
+        <v>266</v>
+      </c>
+      <c r="B135" t="s">
         <v>267</v>
-      </c>
-      <c r="B135" t="s">
-        <v>268</v>
       </c>
       <c r="C135" t="s">
         <v>9</v>
@@ -23155,10 +23140,10 @@
     </row>
     <row r="136" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
+        <v>268</v>
+      </c>
+      <c r="B136" t="s">
         <v>269</v>
-      </c>
-      <c r="B136" t="s">
-        <v>270</v>
       </c>
       <c r="C136" t="s">
         <v>9</v>
@@ -23334,10 +23319,10 @@
     </row>
     <row r="137" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
+        <v>270</v>
+      </c>
+      <c r="B137" t="s">
         <v>271</v>
-      </c>
-      <c r="B137" t="s">
-        <v>272</v>
       </c>
       <c r="C137" t="s">
         <v>9</v>
@@ -23513,10 +23498,10 @@
     </row>
     <row r="138" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
+        <v>272</v>
+      </c>
+      <c r="B138" t="s">
         <v>273</v>
-      </c>
-      <c r="B138" t="s">
-        <v>274</v>
       </c>
       <c r="C138" t="s">
         <v>9</v>
@@ -23692,10 +23677,10 @@
     </row>
     <row r="139" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
+        <v>274</v>
+      </c>
+      <c r="B139" t="s">
         <v>275</v>
-      </c>
-      <c r="B139" t="s">
-        <v>276</v>
       </c>
       <c r="C139" t="s">
         <v>9</v>
@@ -23871,10 +23856,10 @@
     </row>
     <row r="140" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
+        <v>276</v>
+      </c>
+      <c r="B140" t="s">
         <v>277</v>
-      </c>
-      <c r="B140" t="s">
-        <v>278</v>
       </c>
       <c r="C140" t="s">
         <v>9</v>
@@ -24050,10 +24035,10 @@
     </row>
     <row r="141" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
+        <v>278</v>
+      </c>
+      <c r="B141" t="s">
         <v>279</v>
-      </c>
-      <c r="B141" t="s">
-        <v>280</v>
       </c>
       <c r="C141" t="s">
         <v>9</v>
@@ -24088,10 +24073,10 @@
     </row>
     <row r="142" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
+        <v>280</v>
+      </c>
+      <c r="B142" t="s">
         <v>281</v>
-      </c>
-      <c r="B142" t="s">
-        <v>282</v>
       </c>
       <c r="C142" t="s">
         <v>9</v>
@@ -24267,10 +24252,10 @@
     </row>
     <row r="143" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
+        <v>282</v>
+      </c>
+      <c r="B143" t="s">
         <v>283</v>
-      </c>
-      <c r="B143" t="s">
-        <v>284</v>
       </c>
       <c r="C143" t="s">
         <v>9</v>
@@ -24446,10 +24431,10 @@
     </row>
     <row r="144" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
+        <v>284</v>
+      </c>
+      <c r="B144" t="s">
         <v>285</v>
-      </c>
-      <c r="B144" t="s">
-        <v>286</v>
       </c>
       <c r="C144" t="s">
         <v>9</v>
@@ -24625,10 +24610,10 @@
     </row>
     <row r="145" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
+        <v>286</v>
+      </c>
+      <c r="B145" t="s">
         <v>287</v>
-      </c>
-      <c r="B145" t="s">
-        <v>288</v>
       </c>
       <c r="C145" t="s">
         <v>9</v>
@@ -24714,10 +24699,10 @@
     </row>
     <row r="146" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
+        <v>288</v>
+      </c>
+      <c r="B146" t="s">
         <v>289</v>
-      </c>
-      <c r="B146" t="s">
-        <v>290</v>
       </c>
       <c r="C146" t="s">
         <v>9</v>
@@ -24893,10 +24878,10 @@
     </row>
     <row r="147" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
+        <v>290</v>
+      </c>
+      <c r="B147" t="s">
         <v>291</v>
-      </c>
-      <c r="B147" t="s">
-        <v>292</v>
       </c>
       <c r="C147" t="s">
         <v>9</v>
@@ -24976,10 +24961,10 @@
     </row>
     <row r="148" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
+        <v>292</v>
+      </c>
+      <c r="B148" t="s">
         <v>293</v>
-      </c>
-      <c r="B148" t="s">
-        <v>294</v>
       </c>
       <c r="C148" t="s">
         <v>9</v>
@@ -25155,10 +25140,10 @@
     </row>
     <row r="149" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
+        <v>294</v>
+      </c>
+      <c r="B149" t="s">
         <v>295</v>
-      </c>
-      <c r="B149" t="s">
-        <v>296</v>
       </c>
       <c r="C149" t="s">
         <v>9</v>
@@ -25238,10 +25223,10 @@
     </row>
     <row r="150" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
+        <v>296</v>
+      </c>
+      <c r="B150" t="s">
         <v>297</v>
-      </c>
-      <c r="B150" t="s">
-        <v>298</v>
       </c>
       <c r="C150" t="s">
         <v>9</v>
@@ -25417,10 +25402,10 @@
     </row>
     <row r="151" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
+        <v>298</v>
+      </c>
+      <c r="B151" t="s">
         <v>299</v>
-      </c>
-      <c r="B151" t="s">
-        <v>300</v>
       </c>
       <c r="C151" t="s">
         <v>9</v>
@@ -25431,10 +25416,10 @@
     </row>
     <row r="152" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
+        <v>300</v>
+      </c>
+      <c r="B152" t="s">
         <v>301</v>
-      </c>
-      <c r="B152" t="s">
-        <v>302</v>
       </c>
       <c r="C152" t="s">
         <v>9</v>
@@ -25610,10 +25595,10 @@
     </row>
     <row r="153" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
+        <v>302</v>
+      </c>
+      <c r="B153" t="s">
         <v>303</v>
-      </c>
-      <c r="B153" t="s">
-        <v>304</v>
       </c>
       <c r="C153" t="s">
         <v>9</v>
@@ -25624,10 +25609,10 @@
     </row>
     <row r="154" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
+        <v>304</v>
+      </c>
+      <c r="B154" t="s">
         <v>305</v>
-      </c>
-      <c r="B154" t="s">
-        <v>306</v>
       </c>
       <c r="C154" t="s">
         <v>9</v>
@@ -25707,10 +25692,10 @@
     </row>
     <row r="155" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
+        <v>306</v>
+      </c>
+      <c r="B155" t="s">
         <v>307</v>
-      </c>
-      <c r="B155" t="s">
-        <v>308</v>
       </c>
       <c r="C155" t="s">
         <v>9</v>
@@ -25886,10 +25871,10 @@
     </row>
     <row r="156" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
+        <v>308</v>
+      </c>
+      <c r="B156" t="s">
         <v>309</v>
-      </c>
-      <c r="B156" t="s">
-        <v>310</v>
       </c>
       <c r="C156" t="s">
         <v>9</v>
@@ -26032,10 +26017,10 @@
     </row>
     <row r="157" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
+        <v>310</v>
+      </c>
+      <c r="B157" t="s">
         <v>311</v>
-      </c>
-      <c r="B157" t="s">
-        <v>312</v>
       </c>
       <c r="C157" t="s">
         <v>9</v>
@@ -26211,10 +26196,10 @@
     </row>
     <row r="158" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
+        <v>312</v>
+      </c>
+      <c r="B158" t="s">
         <v>313</v>
-      </c>
-      <c r="B158" t="s">
-        <v>314</v>
       </c>
       <c r="C158" t="s">
         <v>9</v>
@@ -26390,10 +26375,10 @@
     </row>
     <row r="159" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
+        <v>314</v>
+      </c>
+      <c r="B159" t="s">
         <v>315</v>
-      </c>
-      <c r="B159" t="s">
-        <v>316</v>
       </c>
       <c r="C159" t="s">
         <v>9</v>
@@ -26479,10 +26464,10 @@
     </row>
     <row r="160" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
+        <v>316</v>
+      </c>
+      <c r="B160" t="s">
         <v>317</v>
-      </c>
-      <c r="B160" t="s">
-        <v>318</v>
       </c>
       <c r="C160" t="s">
         <v>9</v>
@@ -26658,10 +26643,10 @@
     </row>
     <row r="161" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
+        <v>318</v>
+      </c>
+      <c r="B161" t="s">
         <v>319</v>
-      </c>
-      <c r="B161" t="s">
-        <v>320</v>
       </c>
       <c r="C161" t="s">
         <v>9</v>
@@ -26741,10 +26726,10 @@
     </row>
     <row r="162" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
+        <v>320</v>
+      </c>
+      <c r="B162" t="s">
         <v>321</v>
-      </c>
-      <c r="B162" t="s">
-        <v>322</v>
       </c>
       <c r="C162" t="s">
         <v>9</v>
@@ -26920,10 +26905,10 @@
     </row>
     <row r="163" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
+        <v>322</v>
+      </c>
+      <c r="B163" t="s">
         <v>323</v>
-      </c>
-      <c r="B163" t="s">
-        <v>324</v>
       </c>
       <c r="C163" t="s">
         <v>9</v>
@@ -27099,10 +27084,10 @@
     </row>
     <row r="164" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
+        <v>324</v>
+      </c>
+      <c r="B164" t="s">
         <v>325</v>
-      </c>
-      <c r="B164" t="s">
-        <v>326</v>
       </c>
       <c r="C164" t="s">
         <v>9</v>
@@ -27278,10 +27263,10 @@
     </row>
     <row r="165" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
+        <v>326</v>
+      </c>
+      <c r="B165" t="s">
         <v>327</v>
-      </c>
-      <c r="B165" t="s">
-        <v>328</v>
       </c>
       <c r="C165" t="s">
         <v>9</v>
@@ -27457,10 +27442,10 @@
     </row>
     <row r="166" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
+        <v>328</v>
+      </c>
+      <c r="B166" t="s">
         <v>329</v>
-      </c>
-      <c r="B166" t="s">
-        <v>330</v>
       </c>
       <c r="C166" t="s">
         <v>9</v>
@@ -27501,10 +27486,10 @@
     </row>
     <row r="167" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
+        <v>330</v>
+      </c>
+      <c r="B167" t="s">
         <v>331</v>
-      </c>
-      <c r="B167" t="s">
-        <v>332</v>
       </c>
       <c r="C167" t="s">
         <v>9</v>
@@ -27680,10 +27665,10 @@
     </row>
     <row r="168" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
+        <v>332</v>
+      </c>
+      <c r="B168" t="s">
         <v>333</v>
-      </c>
-      <c r="B168" t="s">
-        <v>334</v>
       </c>
       <c r="C168" t="s">
         <v>9</v>
@@ -27694,10 +27679,10 @@
     </row>
     <row r="169" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
+        <v>334</v>
+      </c>
+      <c r="B169" t="s">
         <v>335</v>
-      </c>
-      <c r="B169" t="s">
-        <v>336</v>
       </c>
       <c r="C169" t="s">
         <v>9</v>
@@ -27873,10 +27858,10 @@
     </row>
     <row r="170" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
+        <v>336</v>
+      </c>
+      <c r="B170" t="s">
         <v>337</v>
-      </c>
-      <c r="B170" t="s">
-        <v>338</v>
       </c>
       <c r="C170" t="s">
         <v>9</v>
@@ -28052,10 +28037,10 @@
     </row>
     <row r="171" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
+        <v>338</v>
+      </c>
+      <c r="B171" t="s">
         <v>339</v>
-      </c>
-      <c r="B171" t="s">
-        <v>340</v>
       </c>
       <c r="C171" t="s">
         <v>9</v>
@@ -28231,10 +28216,10 @@
     </row>
     <row r="172" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
+        <v>340</v>
+      </c>
+      <c r="B172" t="s">
         <v>341</v>
-      </c>
-      <c r="B172" t="s">
-        <v>342</v>
       </c>
       <c r="C172" t="s">
         <v>9</v>
@@ -28398,10 +28383,10 @@
     </row>
     <row r="173" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
+        <v>342</v>
+      </c>
+      <c r="B173" t="s">
         <v>343</v>
-      </c>
-      <c r="B173" t="s">
-        <v>344</v>
       </c>
       <c r="C173" t="s">
         <v>9</v>
@@ -28547,10 +28532,10 @@
     </row>
     <row r="174" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
+        <v>344</v>
+      </c>
+      <c r="B174" t="s">
         <v>345</v>
-      </c>
-      <c r="B174" t="s">
-        <v>346</v>
       </c>
       <c r="C174" t="s">
         <v>9</v>
@@ -28726,10 +28711,10 @@
     </row>
     <row r="175" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
+        <v>346</v>
+      </c>
+      <c r="B175" t="s">
         <v>347</v>
-      </c>
-      <c r="B175" t="s">
-        <v>348</v>
       </c>
       <c r="C175" t="s">
         <v>9</v>
@@ -28815,10 +28800,10 @@
     </row>
     <row r="176" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
+        <v>348</v>
+      </c>
+      <c r="B176" t="s">
         <v>349</v>
-      </c>
-      <c r="B176" t="s">
-        <v>350</v>
       </c>
       <c r="C176" t="s">
         <v>9</v>
@@ -28994,10 +28979,10 @@
     </row>
     <row r="177" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
+        <v>350</v>
+      </c>
+      <c r="B177" t="s">
         <v>351</v>
-      </c>
-      <c r="B177" t="s">
-        <v>352</v>
       </c>
       <c r="C177" t="s">
         <v>9</v>
@@ -29173,10 +29158,10 @@
     </row>
     <row r="178" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
+        <v>352</v>
+      </c>
+      <c r="B178" t="s">
         <v>353</v>
-      </c>
-      <c r="B178" t="s">
-        <v>354</v>
       </c>
       <c r="C178" t="s">
         <v>9</v>
@@ -29352,10 +29337,10 @@
     </row>
     <row r="179" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
+        <v>354</v>
+      </c>
+      <c r="B179" t="s">
         <v>355</v>
-      </c>
-      <c r="B179" t="s">
-        <v>356</v>
       </c>
       <c r="C179" t="s">
         <v>9</v>
@@ -29531,10 +29516,10 @@
     </row>
     <row r="180" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
+        <v>356</v>
+      </c>
+      <c r="B180" t="s">
         <v>357</v>
-      </c>
-      <c r="B180" t="s">
-        <v>358</v>
       </c>
       <c r="C180" t="s">
         <v>9</v>
@@ -29710,10 +29695,10 @@
     </row>
     <row r="181" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
+        <v>358</v>
+      </c>
+      <c r="B181" t="s">
         <v>359</v>
-      </c>
-      <c r="B181" t="s">
-        <v>360</v>
       </c>
       <c r="C181" t="s">
         <v>9</v>
@@ -29889,10 +29874,10 @@
     </row>
     <row r="182" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
+        <v>360</v>
+      </c>
+      <c r="B182" t="s">
         <v>361</v>
-      </c>
-      <c r="B182" t="s">
-        <v>362</v>
       </c>
       <c r="C182" t="s">
         <v>9</v>
@@ -30068,10 +30053,10 @@
     </row>
     <row r="183" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
+        <v>362</v>
+      </c>
+      <c r="B183" t="s">
         <v>363</v>
-      </c>
-      <c r="B183" t="s">
-        <v>364</v>
       </c>
       <c r="C183" t="s">
         <v>9</v>
@@ -30235,10 +30220,10 @@
     </row>
     <row r="184" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
+        <v>364</v>
+      </c>
+      <c r="B184" t="s">
         <v>365</v>
-      </c>
-      <c r="B184" t="s">
-        <v>366</v>
       </c>
       <c r="C184" t="s">
         <v>9</v>
@@ -30414,10 +30399,10 @@
     </row>
     <row r="185" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
+        <v>366</v>
+      </c>
+      <c r="B185" t="s">
         <v>367</v>
-      </c>
-      <c r="B185" t="s">
-        <v>368</v>
       </c>
       <c r="C185" t="s">
         <v>9</v>
@@ -30593,10 +30578,10 @@
     </row>
     <row r="186" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
+        <v>368</v>
+      </c>
+      <c r="B186" t="s">
         <v>369</v>
-      </c>
-      <c r="B186" t="s">
-        <v>370</v>
       </c>
       <c r="C186" t="s">
         <v>9</v>
@@ -30760,10 +30745,10 @@
     </row>
     <row r="187" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
+        <v>370</v>
+      </c>
+      <c r="B187" t="s">
         <v>371</v>
-      </c>
-      <c r="B187" t="s">
-        <v>372</v>
       </c>
       <c r="C187" t="s">
         <v>9</v>
@@ -30939,10 +30924,10 @@
     </row>
     <row r="188" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
+        <v>372</v>
+      </c>
+      <c r="B188" t="s">
         <v>373</v>
-      </c>
-      <c r="B188" t="s">
-        <v>374</v>
       </c>
       <c r="C188" t="s">
         <v>9</v>
@@ -31118,10 +31103,10 @@
     </row>
     <row r="189" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
+        <v>374</v>
+      </c>
+      <c r="B189" t="s">
         <v>375</v>
-      </c>
-      <c r="B189" t="s">
-        <v>376</v>
       </c>
       <c r="C189" t="s">
         <v>9</v>
@@ -31297,10 +31282,10 @@
     </row>
     <row r="190" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
+        <v>376</v>
+      </c>
+      <c r="B190" t="s">
         <v>377</v>
-      </c>
-      <c r="B190" t="s">
-        <v>378</v>
       </c>
       <c r="C190" t="s">
         <v>9</v>
@@ -31476,10 +31461,10 @@
     </row>
     <row r="191" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
+        <v>378</v>
+      </c>
+      <c r="B191" t="s">
         <v>379</v>
-      </c>
-      <c r="B191" t="s">
-        <v>380</v>
       </c>
       <c r="C191" t="s">
         <v>9</v>
@@ -31655,10 +31640,10 @@
     </row>
     <row r="192" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
+        <v>380</v>
+      </c>
+      <c r="B192" t="s">
         <v>381</v>
-      </c>
-      <c r="B192" t="s">
-        <v>382</v>
       </c>
       <c r="C192" t="s">
         <v>9</v>
@@ -31834,10 +31819,10 @@
     </row>
     <row r="193" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
+        <v>382</v>
+      </c>
+      <c r="B193" t="s">
         <v>383</v>
-      </c>
-      <c r="B193" t="s">
-        <v>384</v>
       </c>
       <c r="C193" t="s">
         <v>9</v>
@@ -32013,10 +31998,10 @@
     </row>
     <row r="194" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
+        <v>384</v>
+      </c>
+      <c r="B194" t="s">
         <v>385</v>
-      </c>
-      <c r="B194" t="s">
-        <v>386</v>
       </c>
       <c r="C194" t="s">
         <v>9</v>
@@ -32192,10 +32177,10 @@
     </row>
     <row r="195" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
+        <v>386</v>
+      </c>
+      <c r="B195" t="s">
         <v>387</v>
-      </c>
-      <c r="B195" t="s">
-        <v>388</v>
       </c>
       <c r="C195" t="s">
         <v>9</v>
@@ -32371,10 +32356,10 @@
     </row>
     <row r="196" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
+        <v>388</v>
+      </c>
+      <c r="B196" t="s">
         <v>389</v>
-      </c>
-      <c r="B196" t="s">
-        <v>390</v>
       </c>
       <c r="C196" t="s">
         <v>9</v>
@@ -32385,10 +32370,10 @@
     </row>
     <row r="197" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
+        <v>390</v>
+      </c>
+      <c r="B197" t="s">
         <v>391</v>
-      </c>
-      <c r="B197" t="s">
-        <v>392</v>
       </c>
       <c r="C197" t="s">
         <v>9</v>
@@ -32450,10 +32435,10 @@
     </row>
     <row r="198" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
+        <v>392</v>
+      </c>
+      <c r="B198" t="s">
         <v>393</v>
-      </c>
-      <c r="B198" t="s">
-        <v>394</v>
       </c>
       <c r="C198" t="s">
         <v>9</v>
@@ -32629,10 +32614,10 @@
     </row>
     <row r="199" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
+        <v>394</v>
+      </c>
+      <c r="B199" t="s">
         <v>395</v>
-      </c>
-      <c r="B199" t="s">
-        <v>396</v>
       </c>
       <c r="C199" t="s">
         <v>9</v>
@@ -32808,10 +32793,10 @@
     </row>
     <row r="200" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
+        <v>396</v>
+      </c>
+      <c r="B200" t="s">
         <v>397</v>
-      </c>
-      <c r="B200" t="s">
-        <v>398</v>
       </c>
       <c r="C200" t="s">
         <v>9</v>
@@ -32873,10 +32858,10 @@
     </row>
     <row r="201" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
+        <v>398</v>
+      </c>
+      <c r="B201" t="s">
         <v>399</v>
-      </c>
-      <c r="B201" t="s">
-        <v>400</v>
       </c>
       <c r="C201" t="s">
         <v>9</v>
@@ -33052,10 +33037,10 @@
     </row>
     <row r="202" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
+        <v>400</v>
+      </c>
+      <c r="B202" t="s">
         <v>401</v>
-      </c>
-      <c r="B202" t="s">
-        <v>402</v>
       </c>
       <c r="C202" t="s">
         <v>9</v>
@@ -33231,10 +33216,10 @@
     </row>
     <row r="203" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
+        <v>402</v>
+      </c>
+      <c r="B203" t="s">
         <v>403</v>
-      </c>
-      <c r="B203" t="s">
-        <v>404</v>
       </c>
       <c r="C203" t="s">
         <v>9</v>
@@ -33410,10 +33395,10 @@
     </row>
     <row r="204" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
+        <v>404</v>
+      </c>
+      <c r="B204" t="s">
         <v>405</v>
-      </c>
-      <c r="B204" t="s">
-        <v>406</v>
       </c>
       <c r="C204" t="s">
         <v>9</v>
@@ -33589,10 +33574,10 @@
     </row>
     <row r="205" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
+        <v>406</v>
+      </c>
+      <c r="B205" t="s">
         <v>407</v>
-      </c>
-      <c r="B205" t="s">
-        <v>408</v>
       </c>
       <c r="C205" t="s">
         <v>9</v>
@@ -33768,10 +33753,10 @@
     </row>
     <row r="206" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
+        <v>408</v>
+      </c>
+      <c r="B206" t="s">
         <v>409</v>
-      </c>
-      <c r="B206" t="s">
-        <v>410</v>
       </c>
       <c r="C206" t="s">
         <v>9</v>
@@ -33851,10 +33836,10 @@
     </row>
     <row r="207" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
+        <v>410</v>
+      </c>
+      <c r="B207" t="s">
         <v>411</v>
-      </c>
-      <c r="B207" t="s">
-        <v>412</v>
       </c>
       <c r="C207" t="s">
         <v>9</v>
@@ -34030,10 +34015,10 @@
     </row>
     <row r="208" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
+        <v>412</v>
+      </c>
+      <c r="B208" t="s">
         <v>413</v>
-      </c>
-      <c r="B208" t="s">
-        <v>414</v>
       </c>
       <c r="C208" t="s">
         <v>9</v>
@@ -34209,10 +34194,10 @@
     </row>
     <row r="209" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
+        <v>414</v>
+      </c>
+      <c r="B209" t="s">
         <v>415</v>
-      </c>
-      <c r="B209" t="s">
-        <v>416</v>
       </c>
       <c r="C209" t="s">
         <v>9</v>
@@ -34388,10 +34373,10 @@
     </row>
     <row r="210" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
+        <v>416</v>
+      </c>
+      <c r="B210" t="s">
         <v>417</v>
-      </c>
-      <c r="B210" t="s">
-        <v>418</v>
       </c>
       <c r="C210" t="s">
         <v>9</v>
@@ -34579,10 +34564,10 @@
     </row>
     <row r="211" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
+        <v>418</v>
+      </c>
+      <c r="B211" t="s">
         <v>419</v>
-      </c>
-      <c r="B211" t="s">
-        <v>420</v>
       </c>
       <c r="C211" t="s">
         <v>9</v>
@@ -34758,10 +34743,10 @@
     </row>
     <row r="212" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
+        <v>420</v>
+      </c>
+      <c r="B212" t="s">
         <v>421</v>
-      </c>
-      <c r="B212" t="s">
-        <v>422</v>
       </c>
       <c r="C212" t="s">
         <v>9</v>
@@ -34937,10 +34922,10 @@
     </row>
     <row r="213" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
+        <v>422</v>
+      </c>
+      <c r="B213" t="s">
         <v>423</v>
-      </c>
-      <c r="B213" t="s">
-        <v>424</v>
       </c>
       <c r="C213" t="s">
         <v>9</v>
@@ -35116,10 +35101,10 @@
     </row>
     <row r="214" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
+        <v>424</v>
+      </c>
+      <c r="B214" t="s">
         <v>425</v>
-      </c>
-      <c r="B214" t="s">
-        <v>426</v>
       </c>
       <c r="C214" t="s">
         <v>9</v>
@@ -35295,10 +35280,10 @@
     </row>
     <row r="215" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
+        <v>426</v>
+      </c>
+      <c r="B215" t="s">
         <v>427</v>
-      </c>
-      <c r="B215" t="s">
-        <v>428</v>
       </c>
       <c r="C215" t="s">
         <v>9</v>
@@ -35474,10 +35459,10 @@
     </row>
     <row r="216" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
+        <v>428</v>
+      </c>
+      <c r="B216" t="s">
         <v>429</v>
-      </c>
-      <c r="B216" t="s">
-        <v>430</v>
       </c>
       <c r="C216" t="s">
         <v>9</v>
@@ -35488,10 +35473,10 @@
     </row>
     <row r="217" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
+        <v>430</v>
+      </c>
+      <c r="B217" t="s">
         <v>431</v>
-      </c>
-      <c r="B217" t="s">
-        <v>432</v>
       </c>
       <c r="C217" t="s">
         <v>9</v>
@@ -35667,10 +35652,10 @@
     </row>
     <row r="218" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
+        <v>432</v>
+      </c>
+      <c r="B218" t="s">
         <v>433</v>
-      </c>
-      <c r="B218" t="s">
-        <v>434</v>
       </c>
       <c r="C218" t="s">
         <v>9</v>
@@ -35708,10 +35693,10 @@
     </row>
     <row r="219" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
+        <v>434</v>
+      </c>
+      <c r="B219" t="s">
         <v>435</v>
-      </c>
-      <c r="B219" t="s">
-        <v>436</v>
       </c>
       <c r="C219" t="s">
         <v>9</v>
@@ -35887,10 +35872,10 @@
     </row>
     <row r="220" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
+        <v>436</v>
+      </c>
+      <c r="B220" t="s">
         <v>437</v>
-      </c>
-      <c r="B220" t="s">
-        <v>438</v>
       </c>
       <c r="C220" t="s">
         <v>9</v>
@@ -35910,10 +35895,10 @@
     </row>
     <row r="221" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
+        <v>438</v>
+      </c>
+      <c r="B221" t="s">
         <v>439</v>
-      </c>
-      <c r="B221" t="s">
-        <v>440</v>
       </c>
       <c r="C221" t="s">
         <v>9</v>
@@ -36089,10 +36074,10 @@
     </row>
     <row r="222" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
+        <v>440</v>
+      </c>
+      <c r="B222" t="s">
         <v>441</v>
-      </c>
-      <c r="B222" t="s">
-        <v>442</v>
       </c>
       <c r="C222" t="s">
         <v>9</v>
@@ -36268,10 +36253,10 @@
     </row>
     <row r="223" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
+        <v>442</v>
+      </c>
+      <c r="B223" t="s">
         <v>443</v>
-      </c>
-      <c r="B223" t="s">
-        <v>444</v>
       </c>
       <c r="C223" t="s">
         <v>9</v>
@@ -36447,10 +36432,10 @@
     </row>
     <row r="224" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
+        <v>444</v>
+      </c>
+      <c r="B224" t="s">
         <v>445</v>
-      </c>
-      <c r="B224" t="s">
-        <v>446</v>
       </c>
       <c r="C224" t="s">
         <v>9</v>
@@ -36626,10 +36611,10 @@
     </row>
     <row r="225" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
+        <v>446</v>
+      </c>
+      <c r="B225" t="s">
         <v>447</v>
-      </c>
-      <c r="B225" t="s">
-        <v>448</v>
       </c>
       <c r="C225" t="s">
         <v>9</v>
@@ -36709,10 +36694,10 @@
     </row>
     <row r="226" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
+        <v>448</v>
+      </c>
+      <c r="B226" t="s">
         <v>449</v>
-      </c>
-      <c r="B226" t="s">
-        <v>450</v>
       </c>
       <c r="C226" t="s">
         <v>9</v>
@@ -36792,10 +36777,10 @@
     </row>
     <row r="227" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
+        <v>450</v>
+      </c>
+      <c r="B227" t="s">
         <v>451</v>
-      </c>
-      <c r="B227" t="s">
-        <v>452</v>
       </c>
       <c r="C227" t="s">
         <v>9</v>
@@ -36971,10 +36956,10 @@
     </row>
     <row r="228" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
+        <v>452</v>
+      </c>
+      <c r="B228" t="s">
         <v>453</v>
-      </c>
-      <c r="B228" t="s">
-        <v>454</v>
       </c>
       <c r="C228" t="s">
         <v>9</v>
@@ -37144,10 +37129,10 @@
     </row>
     <row r="229" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
+        <v>454</v>
+      </c>
+      <c r="B229" t="s">
         <v>455</v>
-      </c>
-      <c r="B229" t="s">
-        <v>456</v>
       </c>
       <c r="C229" t="s">
         <v>9</v>
@@ -37167,10 +37152,10 @@
     </row>
     <row r="230" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
+        <v>456</v>
+      </c>
+      <c r="B230" t="s">
         <v>457</v>
-      </c>
-      <c r="B230" t="s">
-        <v>458</v>
       </c>
       <c r="C230" t="s">
         <v>9</v>
@@ -37337,10 +37322,10 @@
     </row>
     <row r="231" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
+        <v>458</v>
+      </c>
+      <c r="B231" t="s">
         <v>459</v>
-      </c>
-      <c r="B231" t="s">
-        <v>460</v>
       </c>
       <c r="C231" t="s">
         <v>9</v>
@@ -37516,10 +37501,10 @@
     </row>
     <row r="232" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
+        <v>460</v>
+      </c>
+      <c r="B232" t="s">
         <v>461</v>
-      </c>
-      <c r="B232" t="s">
-        <v>462</v>
       </c>
       <c r="C232" t="s">
         <v>9</v>
@@ -37605,10 +37590,10 @@
     </row>
     <row r="233" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
+        <v>462</v>
+      </c>
+      <c r="B233" t="s">
         <v>463</v>
-      </c>
-      <c r="B233" t="s">
-        <v>464</v>
       </c>
       <c r="C233" t="s">
         <v>9</v>
@@ -37784,10 +37769,10 @@
     </row>
     <row r="234" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
+        <v>464</v>
+      </c>
+      <c r="B234" t="s">
         <v>465</v>
-      </c>
-      <c r="B234" t="s">
-        <v>466</v>
       </c>
       <c r="C234" t="s">
         <v>9</v>
@@ -37963,10 +37948,10 @@
     </row>
     <row r="235" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
+        <v>466</v>
+      </c>
+      <c r="B235" t="s">
         <v>467</v>
-      </c>
-      <c r="B235" t="s">
-        <v>468</v>
       </c>
       <c r="C235" t="s">
         <v>9</v>
@@ -38046,10 +38031,10 @@
     </row>
     <row r="236" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
+        <v>468</v>
+      </c>
+      <c r="B236" t="s">
         <v>469</v>
-      </c>
-      <c r="B236" t="s">
-        <v>470</v>
       </c>
       <c r="C236" t="s">
         <v>9</v>
@@ -38225,10 +38210,10 @@
     </row>
     <row r="237" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
+        <v>470</v>
+      </c>
+      <c r="B237" t="s">
         <v>471</v>
-      </c>
-      <c r="B237" t="s">
-        <v>472</v>
       </c>
       <c r="C237" t="s">
         <v>9</v>
@@ -38404,10 +38389,10 @@
     </row>
     <row r="238" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
+        <v>472</v>
+      </c>
+      <c r="B238" t="s">
         <v>473</v>
-      </c>
-      <c r="B238" t="s">
-        <v>474</v>
       </c>
       <c r="C238" t="s">
         <v>9</v>
@@ -38487,10 +38472,10 @@
     </row>
     <row r="239" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
+        <v>474</v>
+      </c>
+      <c r="B239" t="s">
         <v>475</v>
-      </c>
-      <c r="B239" t="s">
-        <v>476</v>
       </c>
       <c r="C239" t="s">
         <v>9</v>
@@ -38570,10 +38555,10 @@
     </row>
     <row r="240" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
+        <v>476</v>
+      </c>
+      <c r="B240" t="s">
         <v>477</v>
-      </c>
-      <c r="B240" t="s">
-        <v>478</v>
       </c>
       <c r="C240" t="s">
         <v>9</v>
@@ -38749,10 +38734,10 @@
     </row>
     <row r="241" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
+        <v>478</v>
+      </c>
+      <c r="B241" t="s">
         <v>479</v>
-      </c>
-      <c r="B241" t="s">
-        <v>480</v>
       </c>
       <c r="C241" t="s">
         <v>9</v>
@@ -38802,10 +38787,10 @@
     </row>
     <row r="242" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
+        <v>480</v>
+      </c>
+      <c r="B242" t="s">
         <v>481</v>
-      </c>
-      <c r="B242" t="s">
-        <v>482</v>
       </c>
       <c r="C242" t="s">
         <v>9</v>
@@ -38981,10 +38966,10 @@
     </row>
     <row r="243" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
+        <v>482</v>
+      </c>
+      <c r="B243" t="s">
         <v>483</v>
-      </c>
-      <c r="B243" t="s">
-        <v>484</v>
       </c>
       <c r="C243" t="s">
         <v>9</v>
@@ -39160,10 +39145,10 @@
     </row>
     <row r="244" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
+        <v>484</v>
+      </c>
+      <c r="B244" t="s">
         <v>485</v>
-      </c>
-      <c r="B244" t="s">
-        <v>486</v>
       </c>
       <c r="C244" t="s">
         <v>9</v>
@@ -39339,10 +39324,10 @@
     </row>
     <row r="245" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
+        <v>486</v>
+      </c>
+      <c r="B245" t="s">
         <v>487</v>
-      </c>
-      <c r="B245" t="s">
-        <v>488</v>
       </c>
       <c r="C245" t="s">
         <v>9</v>
@@ -39518,10 +39503,10 @@
     </row>
     <row r="246" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
+        <v>488</v>
+      </c>
+      <c r="B246" t="s">
         <v>489</v>
-      </c>
-      <c r="B246" t="s">
-        <v>490</v>
       </c>
       <c r="C246" t="s">
         <v>9</v>
@@ -39697,10 +39682,10 @@
     </row>
     <row r="247" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
+        <v>490</v>
+      </c>
+      <c r="B247" t="s">
         <v>491</v>
-      </c>
-      <c r="B247" t="s">
-        <v>492</v>
       </c>
       <c r="C247" t="s">
         <v>9</v>
@@ -39876,10 +39861,10 @@
     </row>
     <row r="248" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
+        <v>492</v>
+      </c>
+      <c r="B248" t="s">
         <v>493</v>
-      </c>
-      <c r="B248" t="s">
-        <v>494</v>
       </c>
       <c r="C248" t="s">
         <v>9</v>
@@ -40055,10 +40040,10 @@
     </row>
     <row r="249" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
+        <v>494</v>
+      </c>
+      <c r="B249" t="s">
         <v>495</v>
-      </c>
-      <c r="B249" t="s">
-        <v>496</v>
       </c>
       <c r="C249" t="s">
         <v>9</v>
@@ -40144,10 +40129,10 @@
     </row>
     <row r="250" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
+        <v>496</v>
+      </c>
+      <c r="B250" t="s">
         <v>497</v>
-      </c>
-      <c r="B250" t="s">
-        <v>498</v>
       </c>
       <c r="C250" t="s">
         <v>9</v>
@@ -40323,10 +40308,10 @@
     </row>
     <row r="251" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
+        <v>498</v>
+      </c>
+      <c r="B251" t="s">
         <v>499</v>
-      </c>
-      <c r="B251" t="s">
-        <v>500</v>
       </c>
       <c r="C251" t="s">
         <v>9</v>
@@ -40502,10 +40487,10 @@
     </row>
     <row r="252" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
+        <v>500</v>
+      </c>
+      <c r="B252" t="s">
         <v>501</v>
-      </c>
-      <c r="B252" t="s">
-        <v>502</v>
       </c>
       <c r="C252" t="s">
         <v>9</v>
@@ -40585,10 +40570,10 @@
     </row>
     <row r="253" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
+        <v>502</v>
+      </c>
+      <c r="B253" t="s">
         <v>503</v>
-      </c>
-      <c r="B253" t="s">
-        <v>504</v>
       </c>
       <c r="C253" t="s">
         <v>9</v>
@@ -40764,10 +40749,10 @@
     </row>
     <row r="254" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
+        <v>504</v>
+      </c>
+      <c r="B254" t="s">
         <v>505</v>
-      </c>
-      <c r="B254" t="s">
-        <v>506</v>
       </c>
       <c r="C254" t="s">
         <v>9</v>
@@ -40943,10 +40928,10 @@
     </row>
     <row r="255" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
+        <v>506</v>
+      </c>
+      <c r="B255" t="s">
         <v>507</v>
-      </c>
-      <c r="B255" t="s">
-        <v>508</v>
       </c>
       <c r="C255" t="s">
         <v>9</v>
@@ -41122,10 +41107,10 @@
     </row>
     <row r="256" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
+        <v>508</v>
+      </c>
+      <c r="B256" t="s">
         <v>509</v>
-      </c>
-      <c r="B256" t="s">
-        <v>510</v>
       </c>
       <c r="C256" t="s">
         <v>9</v>
@@ -41205,10 +41190,10 @@
     </row>
     <row r="257" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
+        <v>510</v>
+      </c>
+      <c r="B257" t="s">
         <v>511</v>
-      </c>
-      <c r="B257" t="s">
-        <v>512</v>
       </c>
       <c r="C257" t="s">
         <v>9</v>
@@ -41384,10 +41369,10 @@
     </row>
     <row r="258" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
+        <v>512</v>
+      </c>
+      <c r="B258" t="s">
         <v>513</v>
-      </c>
-      <c r="B258" t="s">
-        <v>514</v>
       </c>
       <c r="C258" t="s">
         <v>9</v>
@@ -41563,10 +41548,10 @@
     </row>
     <row r="259" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
+        <v>514</v>
+      </c>
+      <c r="B259" t="s">
         <v>515</v>
-      </c>
-      <c r="B259" t="s">
-        <v>516</v>
       </c>
       <c r="C259" t="s">
         <v>9</v>
@@ -41736,10 +41721,10 @@
     </row>
     <row r="260" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
+        <v>516</v>
+      </c>
+      <c r="B260" t="s">
         <v>517</v>
-      </c>
-      <c r="B260" t="s">
-        <v>518</v>
       </c>
       <c r="C260" t="s">
         <v>9</v>
@@ -41750,10 +41735,10 @@
     </row>
     <row r="261" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
+        <v>518</v>
+      </c>
+      <c r="B261" t="s">
         <v>519</v>
-      </c>
-      <c r="B261" t="s">
-        <v>520</v>
       </c>
       <c r="C261" t="s">
         <v>9</v>
@@ -41929,10 +41914,10 @@
     </row>
     <row r="262" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
+        <v>520</v>
+      </c>
+      <c r="B262" t="s">
         <v>521</v>
-      </c>
-      <c r="B262" t="s">
-        <v>522</v>
       </c>
       <c r="C262" t="s">
         <v>9</v>
@@ -42102,10 +42087,10 @@
     </row>
     <row r="263" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
+        <v>522</v>
+      </c>
+      <c r="B263" t="s">
         <v>523</v>
-      </c>
-      <c r="B263" t="s">
-        <v>524</v>
       </c>
       <c r="C263" t="s">
         <v>9</v>
@@ -42281,10 +42266,10 @@
     </row>
     <row r="264" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
+        <v>524</v>
+      </c>
+      <c r="B264" t="s">
         <v>525</v>
-      </c>
-      <c r="B264" t="s">
-        <v>526</v>
       </c>
       <c r="C264" t="s">
         <v>9</v>
@@ -42460,10 +42445,10 @@
     </row>
     <row r="265" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
+        <v>526</v>
+      </c>
+      <c r="B265" t="s">
         <v>527</v>
-      </c>
-      <c r="B265" t="s">
-        <v>528</v>
       </c>
       <c r="C265" t="s">
         <v>9</v>
@@ -42474,10 +42459,10 @@
     </row>
     <row r="266" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
+        <v>528</v>
+      </c>
+      <c r="B266" t="s">
         <v>529</v>
-      </c>
-      <c r="B266" t="s">
-        <v>530</v>
       </c>
       <c r="C266" t="s">
         <v>9</v>
@@ -42653,10 +42638,10 @@
     </row>
     <row r="267" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
+        <v>530</v>
+      </c>
+      <c r="B267" t="s">
         <v>531</v>
-      </c>
-      <c r="B267" t="s">
-        <v>532</v>
       </c>
       <c r="C267" t="s">
         <v>9</v>
@@ -42832,10 +42817,10 @@
     </row>
     <row r="268" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
+        <v>532</v>
+      </c>
+      <c r="B268" t="s">
         <v>533</v>
-      </c>
-      <c r="B268" t="s">
-        <v>534</v>
       </c>
       <c r="C268" t="s">
         <v>9</v>
@@ -42999,10 +42984,10 @@
     </row>
     <row r="269" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
+        <v>534</v>
+      </c>
+      <c r="B269" t="s">
         <v>535</v>
-      </c>
-      <c r="B269" t="s">
-        <v>536</v>
       </c>
       <c r="C269" t="s">
         <v>9</v>

</xml_diff>